<commit_message>
Update Strategy Script and .gitignore File.
</commit_message>
<xml_diff>
--- a/strategy/2024-04-30.xlsx
+++ b/strategy/2024-04-30.xlsx
@@ -61,9 +61,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="166" formatCode="hh:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -372,7 +372,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1012,7 +1012,7 @@
         <v>45412.9166550926</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>54.2</v>
+        <v>51</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -1039,7 +1039,7 @@
         <v>45412.9583217593</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>54.2</v>
+        <v>51</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -1066,7 +1066,7 @@
         <v>45412.9999884259</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>54.2</v>
+        <v>51</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">$H$3</f>

</xml_diff>